<commit_message>
Subindo Documentação e Backolg de Requisitos
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55119\Documents\SPTECH\EscolinhaDoTom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFEC8BD-CB28-4699-A7AA-88E5368273EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F879C16-3EEA-4702-927A-194A2462805A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07257DC1-4D44-4C39-8168-825E29C32C2B}"/>
   </bookViews>
@@ -307,15 +307,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,17 +336,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,7 +669,7 @@
   <dimension ref="C1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C2" sqref="C2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,47 +689,47 @@
       <c r="E1"/>
     </row>
     <row r="2" spans="3:9" ht="29.4" x14ac:dyDescent="0.45">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="3:9" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -749,13 +746,13 @@
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -772,13 +769,13 @@
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -795,13 +792,13 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -818,13 +815,13 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -841,13 +838,13 @@
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -864,13 +861,13 @@
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -887,13 +884,13 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -910,13 +907,13 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -933,13 +930,13 @@
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -956,13 +953,13 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -979,13 +976,13 @@
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1002,13 +999,13 @@
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -1024,72 +1021,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="H19" s="14" t="s">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="12">
         <f>SUM(G4:G16)</f>
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="H20" s="13" t="s">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="10">
         <f>SUM(G16,G4:G6,G9)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="H21" s="13" t="s">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="10">
         <f>SUM(G7:G8,G10:G11)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="H22" s="13" t="s">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="10">
         <f>SUM(G14:G15,G12:G13)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="H23" s="16" t="s">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="14">
         <f>AVERAGE(I20:I22)</f>
         <v>42.666666666666664</v>
       </c>

</xml_diff>